<commit_message>
continued changes - works at this point
</commit_message>
<xml_diff>
--- a/Shiny_app/FDA_Drug_Trials_Snapshots_2015-20.xlsx
+++ b/Shiny_app/FDA_Drug_Trials_Snapshots_2015-20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Documents/GitHub/FDA_DTS/Shiny_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C52CA6-2BDE-644C-A7D5-460A6D8C3D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EA8ADF6-77EB-2F46-91EC-919AAB9DF5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2845,6 +2845,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3296,7 +3299,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -3339,15 +3342,17 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -3375,6 +3380,7 @@
     <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Comma" xfId="42" builtinId="3"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -3809,7 +3815,7 @@
       <c r="G2" t="s">
         <v>471</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="5">
         <v>2015</v>
       </c>
       <c r="I2">
@@ -3862,7 +3868,7 @@
       <c r="G3" t="s">
         <v>354</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>2015</v>
       </c>
       <c r="I3">
@@ -3915,7 +3921,7 @@
       <c r="G4" t="s">
         <v>55</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>2015</v>
       </c>
       <c r="I4">
@@ -3968,7 +3974,7 @@
       <c r="G5" t="s">
         <v>501</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>2015</v>
       </c>
       <c r="I5">
@@ -4021,7 +4027,7 @@
       <c r="G6" t="s">
         <v>327</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="5">
         <v>2015</v>
       </c>
       <c r="I6">
@@ -4077,7 +4083,7 @@
       <c r="G7" t="s">
         <v>437</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="5">
         <v>2015</v>
       </c>
       <c r="I7">
@@ -4130,7 +4136,7 @@
       <c r="G8" t="s">
         <v>483</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="5">
         <v>2015</v>
       </c>
       <c r="I8">
@@ -4174,7 +4180,7 @@
       <c r="G9" t="s">
         <v>336</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>2015</v>
       </c>
       <c r="I9">
@@ -4218,7 +4224,7 @@
       <c r="G10" t="s">
         <v>392</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="5">
         <v>2015</v>
       </c>
       <c r="I10">
@@ -4271,7 +4277,7 @@
       <c r="G11" t="s">
         <v>394</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>2015</v>
       </c>
       <c r="I11">
@@ -4324,7 +4330,7 @@
       <c r="G12" t="s">
         <v>532</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <v>2015</v>
       </c>
       <c r="I12">
@@ -4371,7 +4377,7 @@
       <c r="G13" t="s">
         <v>507</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <v>2015</v>
       </c>
       <c r="I13">
@@ -4424,7 +4430,7 @@
       <c r="G14" t="s">
         <v>251</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>2015</v>
       </c>
       <c r="I14">
@@ -4477,7 +4483,7 @@
       <c r="G15" t="s">
         <v>396</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>2015</v>
       </c>
       <c r="I15">
@@ -4530,7 +4536,7 @@
       <c r="G16" t="s">
         <v>71</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="5">
         <v>2015</v>
       </c>
       <c r="I16">
@@ -4583,7 +4589,7 @@
       <c r="G17" t="s">
         <v>71</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="5">
         <v>2015</v>
       </c>
       <c r="I17">
@@ -4636,7 +4642,7 @@
       <c r="G18" t="s">
         <v>459</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>2015</v>
       </c>
       <c r="I18">
@@ -4689,7 +4695,7 @@
       <c r="G19" t="s">
         <v>71</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="5">
         <v>2015</v>
       </c>
       <c r="I19">
@@ -4742,7 +4748,7 @@
       <c r="G20" t="s">
         <v>47</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="5">
         <v>2015</v>
       </c>
       <c r="I20">
@@ -4795,7 +4801,7 @@
       <c r="G21" t="s">
         <v>172</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="5">
         <v>2015</v>
       </c>
       <c r="I21">
@@ -4848,7 +4854,7 @@
       <c r="G22" t="s">
         <v>429</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="5">
         <v>2015</v>
       </c>
       <c r="I22">
@@ -4901,7 +4907,7 @@
       <c r="G23" t="s">
         <v>487</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="5">
         <v>2015</v>
       </c>
       <c r="I23">
@@ -4954,7 +4960,7 @@
       <c r="G24" t="s">
         <v>418</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="5">
         <v>2015</v>
       </c>
       <c r="I24">
@@ -5007,7 +5013,7 @@
       <c r="G25" t="s">
         <v>439</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="5">
         <v>2015</v>
       </c>
       <c r="I25">
@@ -5060,7 +5066,7 @@
       <c r="G26" t="s">
         <v>473</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="5">
         <v>2015</v>
       </c>
       <c r="I26">
@@ -5113,7 +5119,7 @@
       <c r="G27" t="s">
         <v>356</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="5">
         <v>2015</v>
       </c>
       <c r="I27">
@@ -5166,7 +5172,7 @@
       <c r="G28" t="s">
         <v>431</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="5">
         <v>2015</v>
       </c>
       <c r="I28">
@@ -5219,7 +5225,7 @@
       <c r="G29" t="s">
         <v>381</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="5">
         <v>2015</v>
       </c>
       <c r="I29">
@@ -5272,7 +5278,7 @@
       <c r="G30" t="s">
         <v>71</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="5">
         <v>2015</v>
       </c>
       <c r="I30">
@@ -5325,7 +5331,7 @@
       <c r="G31" t="s">
         <v>441</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="5">
         <v>2015</v>
       </c>
       <c r="I31">
@@ -5378,7 +5384,7 @@
       <c r="G32" t="s">
         <v>445</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="5">
         <v>2015</v>
       </c>
       <c r="I32">
@@ -5431,7 +5437,7 @@
       <c r="G33" t="s">
         <v>95</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="5">
         <v>2015</v>
       </c>
       <c r="I33">
@@ -5484,7 +5490,7 @@
       <c r="G34" t="s">
         <v>447</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="5">
         <v>2015</v>
       </c>
       <c r="I34">
@@ -5537,7 +5543,7 @@
       <c r="G35" t="s">
         <v>453</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="5">
         <v>2015</v>
       </c>
       <c r="I35">
@@ -5593,7 +5599,7 @@
       <c r="G36" t="s">
         <v>385</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="5">
         <v>2015</v>
       </c>
       <c r="I36">
@@ -5646,7 +5652,7 @@
       <c r="G37" t="s">
         <v>461</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="5">
         <v>2015</v>
       </c>
       <c r="I37">
@@ -5699,7 +5705,7 @@
       <c r="G38" t="s">
         <v>340</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="5">
         <v>2015</v>
       </c>
       <c r="I38">
@@ -5752,7 +5758,7 @@
       <c r="G39" t="s">
         <v>55</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="5">
         <v>2015</v>
       </c>
       <c r="I39">
@@ -5805,7 +5811,7 @@
       <c r="G40" t="s">
         <v>495</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="5">
         <v>2015</v>
       </c>
       <c r="I40">
@@ -5861,7 +5867,7 @@
       <c r="G41" t="s">
         <v>449</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="5">
         <v>2015</v>
       </c>
       <c r="I41">
@@ -5914,7 +5920,7 @@
       <c r="G42" t="s">
         <v>398</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="5">
         <v>2015</v>
       </c>
       <c r="I42">
@@ -5967,7 +5973,7 @@
       <c r="G43" t="s">
         <v>342</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="5">
         <v>2015</v>
       </c>
       <c r="I43">
@@ -6020,7 +6026,7 @@
       <c r="G44" t="s">
         <v>344</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="5">
         <v>2015</v>
       </c>
       <c r="I44">
@@ -6073,7 +6079,7 @@
       <c r="G45" t="s">
         <v>465</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="5">
         <v>2015</v>
       </c>
       <c r="I45">
@@ -6126,7 +6132,7 @@
       <c r="G46" t="s">
         <v>387</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="5">
         <v>2015</v>
       </c>
       <c r="I46">
@@ -6179,7 +6185,7 @@
       <c r="G47" t="s">
         <v>467</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="5">
         <v>2015</v>
       </c>
       <c r="I47">
@@ -6232,7 +6238,7 @@
       <c r="G48" t="s">
         <v>84</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="5">
         <v>2015</v>
       </c>
       <c r="I48">
@@ -6276,7 +6282,7 @@
       <c r="G49" t="s">
         <v>421</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="5">
         <v>2015</v>
       </c>
       <c r="I49">
@@ -6329,7 +6335,7 @@
       <c r="G50" t="s">
         <v>922</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="5">
         <v>2015</v>
       </c>
       <c r="I50">
@@ -6382,7 +6388,7 @@
       <c r="G51" t="s">
         <v>389</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="5">
         <v>2015</v>
       </c>
       <c r="I51">
@@ -6435,7 +6441,7 @@
       <c r="G52" t="s">
         <v>497</v>
       </c>
-      <c r="H52">
+      <c r="H52" s="5">
         <v>2015</v>
       </c>
       <c r="I52">
@@ -6488,7 +6494,7 @@
       <c r="G53" t="s">
         <v>55</v>
       </c>
-      <c r="H53">
+      <c r="H53" s="5">
         <v>2015</v>
       </c>
       <c r="I53">
@@ -6541,7 +6547,7 @@
       <c r="G54" t="s">
         <v>505</v>
       </c>
-      <c r="H54">
+      <c r="H54" s="5">
         <v>2015</v>
       </c>
       <c r="I54">
@@ -6594,7 +6600,7 @@
       <c r="G55" t="s">
         <v>346</v>
       </c>
-      <c r="H55">
+      <c r="H55" s="5">
         <v>2015</v>
       </c>
       <c r="I55">
@@ -6638,7 +6644,7 @@
       <c r="G56" t="s">
         <v>51</v>
       </c>
-      <c r="H56">
+      <c r="H56" s="5">
         <v>2015</v>
       </c>
       <c r="I56">
@@ -6691,7 +6697,7 @@
       <c r="G57" t="s">
         <v>490</v>
       </c>
-      <c r="H57">
+      <c r="H57" s="5">
         <v>2015</v>
       </c>
       <c r="I57">
@@ -6744,7 +6750,7 @@
       <c r="G58" t="s">
         <v>433</v>
       </c>
-      <c r="H58">
+      <c r="H58" s="5">
         <v>2016</v>
       </c>
       <c r="I58">
@@ -6791,7 +6797,7 @@
       <c r="G59" t="s">
         <v>443</v>
       </c>
-      <c r="H59">
+      <c r="H59" s="5">
         <v>2016</v>
       </c>
       <c r="I59">
@@ -6838,7 +6844,7 @@
       <c r="G60" t="s">
         <v>170</v>
       </c>
-      <c r="H60">
+      <c r="H60" s="5">
         <v>2016</v>
       </c>
       <c r="I60">
@@ -6885,7 +6891,7 @@
       <c r="G61" t="s">
         <v>142</v>
       </c>
-      <c r="H61">
+      <c r="H61" s="5">
         <v>2016</v>
       </c>
       <c r="I61">
@@ -6932,7 +6938,7 @@
       <c r="G62" t="s">
         <v>236</v>
       </c>
-      <c r="H62">
+      <c r="H62" s="5">
         <v>2016</v>
       </c>
       <c r="I62">
@@ -6979,7 +6985,7 @@
       <c r="G63" t="s">
         <v>441</v>
       </c>
-      <c r="H63">
+      <c r="H63" s="5">
         <v>2016</v>
       </c>
       <c r="I63">
@@ -7026,7 +7032,7 @@
       <c r="G64" t="s">
         <v>107</v>
       </c>
-      <c r="H64">
+      <c r="H64" s="5">
         <v>2016</v>
       </c>
       <c r="I64">
@@ -7073,7 +7079,7 @@
       <c r="G65" t="s">
         <v>298</v>
       </c>
-      <c r="H65">
+      <c r="H65" s="5">
         <v>2016</v>
       </c>
       <c r="I65">
@@ -7120,7 +7126,7 @@
       <c r="G66" t="s">
         <v>509</v>
       </c>
-      <c r="H66">
+      <c r="H66" s="5">
         <v>2016</v>
       </c>
       <c r="I66">
@@ -7167,7 +7173,7 @@
       <c r="G67" t="s">
         <v>333</v>
       </c>
-      <c r="H67">
+      <c r="H67" s="5">
         <v>2016</v>
       </c>
       <c r="I67">
@@ -7214,7 +7220,7 @@
       <c r="G68" t="s">
         <v>333</v>
       </c>
-      <c r="H68">
+      <c r="H68" s="5">
         <v>2016</v>
       </c>
       <c r="I68">
@@ -7261,7 +7267,7 @@
       <c r="G69" t="s">
         <v>80</v>
       </c>
-      <c r="H69">
+      <c r="H69" s="5">
         <v>2016</v>
       </c>
       <c r="I69">
@@ -7308,7 +7314,7 @@
       <c r="G70" t="s">
         <v>530</v>
       </c>
-      <c r="H70">
+      <c r="H70" s="5">
         <v>2016</v>
       </c>
       <c r="I70">
@@ -7346,7 +7352,7 @@
       <c r="G71" t="s">
         <v>372</v>
       </c>
-      <c r="H71">
+      <c r="H71" s="5">
         <v>2016</v>
       </c>
       <c r="I71">
@@ -7393,7 +7399,7 @@
       <c r="G72" t="s">
         <v>374</v>
       </c>
-      <c r="H72">
+      <c r="H72" s="5">
         <v>2016</v>
       </c>
       <c r="I72">
@@ -7440,7 +7446,7 @@
       <c r="G73" t="s">
         <v>350</v>
       </c>
-      <c r="H73">
+      <c r="H73" s="5">
         <v>2016</v>
       </c>
       <c r="I73">
@@ -7487,7 +7493,7 @@
       <c r="G74" t="s">
         <v>414</v>
       </c>
-      <c r="H74">
+      <c r="H74" s="5">
         <v>2016</v>
       </c>
       <c r="I74">
@@ -7534,7 +7540,7 @@
       <c r="G75" t="s">
         <v>416</v>
       </c>
-      <c r="H75">
+      <c r="H75" s="5">
         <v>2016</v>
       </c>
       <c r="I75">
@@ -7581,7 +7587,7 @@
       <c r="G76" t="s">
         <v>352</v>
       </c>
-      <c r="H76">
+      <c r="H76" s="5">
         <v>2016</v>
       </c>
       <c r="I76">
@@ -7628,7 +7634,7 @@
       <c r="G77" t="s">
         <v>219</v>
       </c>
-      <c r="H77">
+      <c r="H77" s="5">
         <v>2016</v>
       </c>
       <c r="I77">
@@ -7675,7 +7681,7 @@
       <c r="G78" t="s">
         <v>479</v>
       </c>
-      <c r="H78">
+      <c r="H78" s="5">
         <v>2016</v>
       </c>
       <c r="I78">
@@ -7722,7 +7728,7 @@
       <c r="G79" t="s">
         <v>183</v>
       </c>
-      <c r="H79">
+      <c r="H79" s="5">
         <v>2016</v>
       </c>
       <c r="I79">
@@ -7769,7 +7775,7 @@
       <c r="G80" t="s">
         <v>376</v>
       </c>
-      <c r="H80">
+      <c r="H80" s="5">
         <v>2016</v>
       </c>
       <c r="I80">
@@ -7816,7 +7822,7 @@
       <c r="G81" t="s">
         <v>317</v>
       </c>
-      <c r="H81">
+      <c r="H81" s="5">
         <v>2016</v>
       </c>
       <c r="I81">
@@ -7863,7 +7869,7 @@
       <c r="G82" t="s">
         <v>469</v>
       </c>
-      <c r="H82">
+      <c r="H82" s="5">
         <v>2017</v>
       </c>
       <c r="I82">
@@ -7913,7 +7919,7 @@
       <c r="G83" t="s">
         <v>404</v>
       </c>
-      <c r="H83">
+      <c r="H83" s="5">
         <v>2017</v>
       </c>
       <c r="I83">
@@ -7960,7 +7966,7 @@
       <c r="G84" t="s">
         <v>39</v>
       </c>
-      <c r="H84">
+      <c r="H84" s="5">
         <v>2017</v>
       </c>
       <c r="I84">
@@ -8010,7 +8016,7 @@
       <c r="G85" t="s">
         <v>475</v>
       </c>
-      <c r="H85">
+      <c r="H85" s="5">
         <v>2017</v>
       </c>
       <c r="I85">
@@ -8060,7 +8066,7 @@
       <c r="G86" t="s">
         <v>307</v>
       </c>
-      <c r="H86">
+      <c r="H86" s="5">
         <v>2017</v>
       </c>
       <c r="I86">
@@ -8110,7 +8116,7 @@
       <c r="G87" t="s">
         <v>528</v>
       </c>
-      <c r="H87">
+      <c r="H87" s="5">
         <v>2017</v>
       </c>
       <c r="I87">
@@ -8148,7 +8154,7 @@
       <c r="G88" t="s">
         <v>266</v>
       </c>
-      <c r="H88">
+      <c r="H88" s="5">
         <v>2017</v>
       </c>
       <c r="I88">
@@ -8195,7 +8201,7 @@
       <c r="G89" t="s">
         <v>215</v>
       </c>
-      <c r="H89">
+      <c r="H89" s="5">
         <v>2017</v>
       </c>
       <c r="I89">
@@ -8245,7 +8251,7 @@
       <c r="G90" t="s">
         <v>121</v>
       </c>
-      <c r="H90">
+      <c r="H90" s="5">
         <v>2017</v>
       </c>
       <c r="I90">
@@ -8295,7 +8301,7 @@
       <c r="G91" t="s">
         <v>157</v>
       </c>
-      <c r="H91">
+      <c r="H91" s="5">
         <v>2017</v>
       </c>
       <c r="I91">
@@ -8345,7 +8351,7 @@
       <c r="G92" t="s">
         <v>128</v>
       </c>
-      <c r="H92">
+      <c r="H92" s="5">
         <v>2017</v>
       </c>
       <c r="I92">
@@ -8395,7 +8401,7 @@
       <c r="G93" t="s">
         <v>331</v>
       </c>
-      <c r="H93">
+      <c r="H93" s="5">
         <v>2017</v>
       </c>
       <c r="I93">
@@ -8439,7 +8445,7 @@
       <c r="G94" t="s">
         <v>283</v>
       </c>
-      <c r="H94">
+      <c r="H94" s="5">
         <v>2017</v>
       </c>
       <c r="I94">
@@ -8492,7 +8498,7 @@
       <c r="G95" t="s">
         <v>259</v>
       </c>
-      <c r="H95">
+      <c r="H95" s="5">
         <v>2017</v>
       </c>
       <c r="I95">
@@ -8542,7 +8548,7 @@
       <c r="G96" t="s">
         <v>234</v>
       </c>
-      <c r="H96">
+      <c r="H96" s="5">
         <v>2017</v>
       </c>
       <c r="I96">
@@ -8592,7 +8598,7 @@
       <c r="G97" t="s">
         <v>105</v>
       </c>
-      <c r="H97">
+      <c r="H97" s="5">
         <v>2017</v>
       </c>
       <c r="I97">
@@ -8642,7 +8648,7 @@
       <c r="G98" t="s">
         <v>212</v>
       </c>
-      <c r="H98">
+      <c r="H98" s="5">
         <v>2017</v>
       </c>
       <c r="I98">
@@ -8689,7 +8695,7 @@
       <c r="G99" t="s">
         <v>309</v>
       </c>
-      <c r="H99">
+      <c r="H99" s="5">
         <v>2017</v>
       </c>
       <c r="I99">
@@ -8739,7 +8745,7 @@
       <c r="G100" t="s">
         <v>321</v>
       </c>
-      <c r="H100">
+      <c r="H100" s="5">
         <v>2017</v>
       </c>
       <c r="I100">
@@ -8789,7 +8795,7 @@
       <c r="G101" t="s">
         <v>189</v>
       </c>
-      <c r="H101">
+      <c r="H101" s="5">
         <v>2017</v>
       </c>
       <c r="I101">
@@ -8839,7 +8845,7 @@
       <c r="G102" t="s">
         <v>413</v>
       </c>
-      <c r="H102">
+      <c r="H102" s="5">
         <v>2017</v>
       </c>
       <c r="I102">
@@ -8886,7 +8892,7 @@
       <c r="G103" t="s">
         <v>273</v>
       </c>
-      <c r="H103">
+      <c r="H103" s="5">
         <v>2017</v>
       </c>
       <c r="I103">
@@ -8936,7 +8942,7 @@
       <c r="G104" t="s">
         <v>324</v>
       </c>
-      <c r="H104">
+      <c r="H104" s="5">
         <v>2017</v>
       </c>
       <c r="I104">
@@ -8986,7 +8992,7 @@
       <c r="G105" t="s">
         <v>146</v>
       </c>
-      <c r="H105">
+      <c r="H105" s="5">
         <v>2017</v>
       </c>
       <c r="I105">
@@ -9036,7 +9042,7 @@
       <c r="G106" t="s">
         <v>223</v>
       </c>
-      <c r="H106">
+      <c r="H106" s="5">
         <v>2017</v>
       </c>
       <c r="I106">
@@ -9086,7 +9092,7 @@
       <c r="G107" t="s">
         <v>264</v>
       </c>
-      <c r="H107">
+      <c r="H107" s="5">
         <v>2017</v>
       </c>
       <c r="I107">
@@ -9136,7 +9142,7 @@
       <c r="G108" t="s">
         <v>242</v>
       </c>
-      <c r="H108">
+      <c r="H108" s="5">
         <v>2017</v>
       </c>
       <c r="I108">
@@ -9186,7 +9192,7 @@
       <c r="G109" t="s">
         <v>455</v>
       </c>
-      <c r="H109">
+      <c r="H109" s="5">
         <v>2017</v>
       </c>
       <c r="I109">
@@ -9236,7 +9242,7 @@
       <c r="G110" t="s">
         <v>24</v>
       </c>
-      <c r="H110">
+      <c r="H110" s="5">
         <v>2017</v>
       </c>
       <c r="I110">
@@ -9286,7 +9292,7 @@
       <c r="G111" t="s">
         <v>282</v>
       </c>
-      <c r="H111">
+      <c r="H111" s="5">
         <v>2017</v>
       </c>
       <c r="I111">
@@ -9336,7 +9342,7 @@
       <c r="G112" t="s">
         <v>232</v>
       </c>
-      <c r="H112">
+      <c r="H112" s="5">
         <v>2017</v>
       </c>
       <c r="I112">
@@ -9386,7 +9392,7 @@
       <c r="G113" t="s">
         <v>367</v>
       </c>
-      <c r="H113">
+      <c r="H113" s="5">
         <v>2017</v>
       </c>
       <c r="I113">
@@ -9436,7 +9442,7 @@
       <c r="G114" t="s">
         <v>159</v>
       </c>
-      <c r="H114">
+      <c r="H114" s="5">
         <v>2017</v>
       </c>
       <c r="I114">
@@ -9483,7 +9489,7 @@
       <c r="G115" t="s">
         <v>78</v>
       </c>
-      <c r="H115">
+      <c r="H115" s="5">
         <v>2017</v>
       </c>
       <c r="I115">
@@ -9533,7 +9539,7 @@
       <c r="G116" t="s">
         <v>264</v>
       </c>
-      <c r="H116">
+      <c r="H116" s="5">
         <v>2017</v>
       </c>
       <c r="I116">
@@ -9583,7 +9589,7 @@
       <c r="G117" t="s">
         <v>187</v>
       </c>
-      <c r="H117">
+      <c r="H117" s="5">
         <v>2017</v>
       </c>
       <c r="I117">
@@ -9633,7 +9639,7 @@
       <c r="G118" t="s">
         <v>159</v>
       </c>
-      <c r="H118">
+      <c r="H118" s="5">
         <v>2017</v>
       </c>
       <c r="I118">
@@ -9683,7 +9689,7 @@
       <c r="G119" t="s">
         <v>596</v>
       </c>
-      <c r="H119">
+      <c r="H119" s="5">
         <v>2017</v>
       </c>
       <c r="I119">
@@ -9733,7 +9739,7 @@
       <c r="G120" t="s">
         <v>291</v>
       </c>
-      <c r="H120">
+      <c r="H120" s="5">
         <v>2017</v>
       </c>
       <c r="I120">
@@ -9783,7 +9789,7 @@
       <c r="G121" t="s">
         <v>499</v>
       </c>
-      <c r="H121">
+      <c r="H121" s="5">
         <v>2017</v>
       </c>
       <c r="I121">
@@ -9833,7 +9839,7 @@
       <c r="G122" t="s">
         <v>189</v>
       </c>
-      <c r="H122">
+      <c r="H122" s="5">
         <v>2017</v>
       </c>
       <c r="I122">
@@ -9883,7 +9889,7 @@
       <c r="G123" t="s">
         <v>197</v>
       </c>
-      <c r="H123">
+      <c r="H123" s="5">
         <v>2017</v>
       </c>
       <c r="I123">
@@ -9933,7 +9939,7 @@
       <c r="G124" t="s">
         <v>238</v>
       </c>
-      <c r="H124">
+      <c r="H124" s="5">
         <v>2017</v>
       </c>
       <c r="I124">
@@ -9983,7 +9989,7 @@
       <c r="G125" t="s">
         <v>60</v>
       </c>
-      <c r="H125">
+      <c r="H125" s="5">
         <v>2017</v>
       </c>
       <c r="I125">
@@ -10033,7 +10039,7 @@
       <c r="G126" t="s">
         <v>82</v>
       </c>
-      <c r="H126">
+      <c r="H126" s="5">
         <v>2017</v>
       </c>
       <c r="I126">
@@ -10086,7 +10092,7 @@
       <c r="G127" t="s">
         <v>36</v>
       </c>
-      <c r="H127">
+      <c r="H127" s="5">
         <v>2017</v>
       </c>
       <c r="I127">
@@ -10136,7 +10142,7 @@
       <c r="G128" t="s">
         <v>369</v>
       </c>
-      <c r="H128">
+      <c r="H128" s="5">
         <v>2017</v>
       </c>
       <c r="I128">
@@ -10186,7 +10192,7 @@
       <c r="G129" t="s">
         <v>463</v>
       </c>
-      <c r="H129">
+      <c r="H129" s="5">
         <v>2018</v>
       </c>
       <c r="I129">
@@ -10248,7 +10254,7 @@
       <c r="G130" t="s">
         <v>168</v>
       </c>
-      <c r="H130">
+      <c r="H130" s="5">
         <v>2018</v>
       </c>
       <c r="I130">
@@ -10310,7 +10316,7 @@
       <c r="G131" t="s">
         <v>168</v>
       </c>
-      <c r="H131">
+      <c r="H131" s="5">
         <v>2018</v>
       </c>
       <c r="I131">
@@ -10375,7 +10381,7 @@
       <c r="G132" t="s">
         <v>360</v>
       </c>
-      <c r="H132">
+      <c r="H132" s="5">
         <v>2018</v>
       </c>
       <c r="I132">
@@ -10434,7 +10440,7 @@
       <c r="G133" t="s">
         <v>313</v>
       </c>
-      <c r="H133">
+      <c r="H133" s="5">
         <v>2018</v>
       </c>
       <c r="I133">
@@ -10496,7 +10502,7 @@
       <c r="G134" t="s">
         <v>125</v>
       </c>
-      <c r="H134">
+      <c r="H134" s="5">
         <v>2018</v>
       </c>
       <c r="I134">
@@ -10558,7 +10564,7 @@
       <c r="G135" t="s">
         <v>140</v>
       </c>
-      <c r="H135">
+      <c r="H135" s="5">
         <v>2018</v>
       </c>
       <c r="I135">
@@ -10620,7 +10626,7 @@
       <c r="G136" t="s">
         <v>481</v>
       </c>
-      <c r="H136">
+      <c r="H136" s="5">
         <v>2018</v>
       </c>
       <c r="I136">
@@ -10682,7 +10688,7 @@
       <c r="G137" t="s">
         <v>191</v>
       </c>
-      <c r="H137">
+      <c r="H137" s="5">
         <v>2018</v>
       </c>
       <c r="I137">
@@ -10744,7 +10750,7 @@
       <c r="G138" t="s">
         <v>181</v>
       </c>
-      <c r="H138">
+      <c r="H138" s="5">
         <v>2018</v>
       </c>
       <c r="I138">
@@ -10806,7 +10812,7 @@
       <c r="G139" t="s">
         <v>411</v>
       </c>
-      <c r="H139">
+      <c r="H139" s="5">
         <v>2018</v>
       </c>
       <c r="I139">
@@ -10865,7 +10871,7 @@
       <c r="G140" t="s">
         <v>526</v>
       </c>
-      <c r="H140">
+      <c r="H140" s="5">
         <v>2018</v>
       </c>
       <c r="I140">
@@ -10915,7 +10921,7 @@
       <c r="G141" t="s">
         <v>176</v>
       </c>
-      <c r="H141">
+      <c r="H141" s="5">
         <v>2018</v>
       </c>
       <c r="I141">
@@ -10977,7 +10983,7 @@
       <c r="G142" t="s">
         <v>138</v>
       </c>
-      <c r="H142">
+      <c r="H142" s="5">
         <v>2018</v>
       </c>
       <c r="I142">
@@ -11039,7 +11045,7 @@
       <c r="G143" t="s">
         <v>168</v>
       </c>
-      <c r="H143">
+      <c r="H143" s="5">
         <v>2018</v>
       </c>
       <c r="I143">
@@ -11101,7 +11107,7 @@
       <c r="G144" t="s">
         <v>76</v>
       </c>
-      <c r="H144">
+      <c r="H144" s="5">
         <v>2018</v>
       </c>
       <c r="I144">
@@ -11163,7 +11169,7 @@
       <c r="G145" t="s">
         <v>87</v>
       </c>
-      <c r="H145">
+      <c r="H145" s="5">
         <v>2018</v>
       </c>
       <c r="I145">
@@ -11225,7 +11231,7 @@
       <c r="G146" t="s">
         <v>240</v>
       </c>
-      <c r="H146">
+      <c r="H146" s="5">
         <v>2018</v>
       </c>
       <c r="I146">
@@ -11287,7 +11293,7 @@
       <c r="G147" t="s">
         <v>148</v>
       </c>
-      <c r="H147">
+      <c r="H147" s="5">
         <v>2018</v>
       </c>
       <c r="I147">
@@ -11349,7 +11355,7 @@
       <c r="G148" t="s">
         <v>477</v>
       </c>
-      <c r="H148">
+      <c r="H148" s="5">
         <v>2018</v>
       </c>
       <c r="I148">
@@ -11408,7 +11414,7 @@
       <c r="G149" t="s">
         <v>195</v>
       </c>
-      <c r="H149">
+      <c r="H149" s="5">
         <v>2018</v>
       </c>
       <c r="I149">
@@ -11470,7 +11476,7 @@
       <c r="G150" t="s">
         <v>227</v>
       </c>
-      <c r="H150">
+      <c r="H150" s="5">
         <v>2018</v>
       </c>
       <c r="I150">
@@ -11532,7 +11538,7 @@
       <c r="G151" t="s">
         <v>366</v>
       </c>
-      <c r="H151">
+      <c r="H151" s="5">
         <v>2018</v>
       </c>
       <c r="I151">
@@ -11594,7 +11600,7 @@
       <c r="G152" t="s">
         <v>315</v>
       </c>
-      <c r="H152">
+      <c r="H152" s="5">
         <v>2018</v>
       </c>
       <c r="I152">
@@ -11656,7 +11662,7 @@
       <c r="G153" t="s">
         <v>426</v>
       </c>
-      <c r="H153">
+      <c r="H153" s="5">
         <v>2018</v>
       </c>
       <c r="I153">
@@ -11718,7 +11724,7 @@
       <c r="G154" t="s">
         <v>271</v>
       </c>
-      <c r="H154">
+      <c r="H154" s="5">
         <v>2018</v>
       </c>
       <c r="I154">
@@ -11780,7 +11786,7 @@
       <c r="G155" t="s">
         <v>402</v>
       </c>
-      <c r="H155">
+      <c r="H155" s="5">
         <v>2018</v>
       </c>
       <c r="I155">
@@ -11842,7 +11848,7 @@
       <c r="G156" t="s">
         <v>137</v>
       </c>
-      <c r="H156">
+      <c r="H156" s="5">
         <v>2018</v>
       </c>
       <c r="I156">
@@ -11904,7 +11910,7 @@
       <c r="G157" t="s">
         <v>492</v>
       </c>
-      <c r="H157">
+      <c r="H157" s="5">
         <v>2018</v>
       </c>
       <c r="I157">
@@ -11966,7 +11972,7 @@
       <c r="G158" t="s">
         <v>424</v>
       </c>
-      <c r="H158">
+      <c r="H158" s="5">
         <v>2018</v>
       </c>
       <c r="I158">
@@ -12025,7 +12031,7 @@
       <c r="G159" t="s">
         <v>44</v>
       </c>
-      <c r="H159">
+      <c r="H159" s="5">
         <v>2018</v>
       </c>
       <c r="I159">
@@ -12087,7 +12093,7 @@
       <c r="G160" t="s">
         <v>176</v>
       </c>
-      <c r="H160">
+      <c r="H160" s="5">
         <v>2018</v>
       </c>
       <c r="I160">
@@ -12149,7 +12155,7 @@
       <c r="G161" t="s">
         <v>378</v>
       </c>
-      <c r="H161">
+      <c r="H161" s="5">
         <v>2018</v>
       </c>
       <c r="I161">
@@ -12211,7 +12217,7 @@
       <c r="G162" t="s">
         <v>451</v>
       </c>
-      <c r="H162">
+      <c r="H162" s="5">
         <v>2018</v>
       </c>
       <c r="I162">
@@ -12273,7 +12279,7 @@
       <c r="G163" t="s">
         <v>296</v>
       </c>
-      <c r="H163">
+      <c r="H163" s="5">
         <v>2018</v>
       </c>
       <c r="I163">
@@ -12338,7 +12344,7 @@
       <c r="G164" t="s">
         <v>286</v>
       </c>
-      <c r="H164">
+      <c r="H164" s="5">
         <v>2018</v>
       </c>
       <c r="I164">
@@ -12400,7 +12406,7 @@
       <c r="G165" t="s">
         <v>230</v>
       </c>
-      <c r="H165">
+      <c r="H165" s="5">
         <v>2018</v>
       </c>
       <c r="I165">
@@ -12462,7 +12468,7 @@
       <c r="G166" t="s">
         <v>253</v>
       </c>
-      <c r="H166">
+      <c r="H166" s="5">
         <v>2018</v>
       </c>
       <c r="I166">
@@ -12524,7 +12530,7 @@
       <c r="G167" t="s">
         <v>207</v>
       </c>
-      <c r="H167">
+      <c r="H167" s="5">
         <v>2018</v>
       </c>
       <c r="I167">
@@ -12583,7 +12589,7 @@
       <c r="G168" t="s">
         <v>92</v>
       </c>
-      <c r="H168">
+      <c r="H168" s="5">
         <v>2018</v>
       </c>
       <c r="I168">
@@ -12645,7 +12651,7 @@
       <c r="G169" t="s">
         <v>178</v>
       </c>
-      <c r="H169">
+      <c r="H169" s="5">
         <v>2018</v>
       </c>
       <c r="I169">
@@ -12707,7 +12713,7 @@
       <c r="G170" t="s">
         <v>67</v>
       </c>
-      <c r="H170">
+      <c r="H170" s="5">
         <v>2018</v>
       </c>
       <c r="I170">
@@ -12769,7 +12775,7 @@
       <c r="G171" t="s">
         <v>311</v>
       </c>
-      <c r="H171">
+      <c r="H171" s="5">
         <v>2018</v>
       </c>
       <c r="I171">
@@ -12831,7 +12837,7 @@
       <c r="G172" t="s">
         <v>302</v>
       </c>
-      <c r="H172">
+      <c r="H172" s="5">
         <v>2018</v>
       </c>
       <c r="I172">
@@ -12893,7 +12899,7 @@
       <c r="G173" t="s">
         <v>95</v>
       </c>
-      <c r="H173">
+      <c r="H173" s="5">
         <v>2018</v>
       </c>
       <c r="I173">
@@ -12958,7 +12964,7 @@
       <c r="G174" t="s">
         <v>131</v>
       </c>
-      <c r="H174">
+      <c r="H174" s="5">
         <v>2018</v>
       </c>
       <c r="I174">
@@ -13020,7 +13026,7 @@
       <c r="G175" t="s">
         <v>199</v>
       </c>
-      <c r="H175">
+      <c r="H175" s="5">
         <v>2018</v>
       </c>
       <c r="I175">
@@ -13082,7 +13088,7 @@
       <c r="G176" t="s">
         <v>100</v>
       </c>
-      <c r="H176">
+      <c r="H176" s="5">
         <v>2018</v>
       </c>
       <c r="I176">
@@ -13144,7 +13150,7 @@
       <c r="G177" t="s">
         <v>246</v>
       </c>
-      <c r="H177">
+      <c r="H177" s="5">
         <v>2018</v>
       </c>
       <c r="I177">
@@ -13206,7 +13212,7 @@
       <c r="G178" t="s">
         <v>103</v>
       </c>
-      <c r="H178">
+      <c r="H178" s="5">
         <v>2018</v>
       </c>
       <c r="I178">
@@ -13268,7 +13274,7 @@
       <c r="G179" t="s">
         <v>151</v>
       </c>
-      <c r="H179">
+      <c r="H179" s="5">
         <v>2018</v>
       </c>
       <c r="I179">
@@ -13330,7 +13336,7 @@
       <c r="G180" t="s">
         <v>97</v>
       </c>
-      <c r="H180">
+      <c r="H180" s="5">
         <v>2018</v>
       </c>
       <c r="I180">
@@ -13392,7 +13398,7 @@
       <c r="G181" t="s">
         <v>161</v>
       </c>
-      <c r="H181">
+      <c r="H181" s="5">
         <v>2018</v>
       </c>
       <c r="I181">
@@ -13454,7 +13460,7 @@
       <c r="G182" t="s">
         <v>73</v>
       </c>
-      <c r="H182">
+      <c r="H182" s="5">
         <v>2018</v>
       </c>
       <c r="I182">
@@ -13516,7 +13522,7 @@
       <c r="G183" t="s">
         <v>363</v>
       </c>
-      <c r="H183">
+      <c r="H183" s="5">
         <v>2018</v>
       </c>
       <c r="I183">
@@ -13578,7 +13584,7 @@
       <c r="G184" t="s">
         <v>457</v>
       </c>
-      <c r="H184">
+      <c r="H184" s="5">
         <v>2018</v>
       </c>
       <c r="I184">
@@ -13640,7 +13646,7 @@
       <c r="G185" t="s">
         <v>289</v>
       </c>
-      <c r="H185">
+      <c r="H185" s="5">
         <v>2018</v>
       </c>
       <c r="I185">
@@ -13702,7 +13708,7 @@
       <c r="G186" t="s">
         <v>111</v>
       </c>
-      <c r="H186">
+      <c r="H186" s="5">
         <v>2018</v>
       </c>
       <c r="I186">
@@ -13764,7 +13770,7 @@
       <c r="G187" t="s">
         <v>133</v>
       </c>
-      <c r="H187">
+      <c r="H187" s="5">
         <v>2018</v>
       </c>
       <c r="I187">
@@ -13826,7 +13832,7 @@
       <c r="G188" t="s">
         <v>513</v>
       </c>
-      <c r="H188">
+      <c r="H188" s="5">
         <v>2018</v>
       </c>
       <c r="I188">
@@ -13888,7 +13894,7 @@
       <c r="G189" t="s">
         <v>166</v>
       </c>
-      <c r="H189">
+      <c r="H189" s="5">
         <v>2019</v>
       </c>
       <c r="I189">
@@ -13950,7 +13956,7 @@
       <c r="G190" t="s">
         <v>29</v>
       </c>
-      <c r="H190">
+      <c r="H190" s="5">
         <v>2019</v>
       </c>
       <c r="I190">
@@ -14009,7 +14015,7 @@
       <c r="G191" t="s">
         <v>185</v>
       </c>
-      <c r="H191">
+      <c r="H191" s="5">
         <v>2019</v>
       </c>
       <c r="I191">
@@ -14071,7 +14077,7 @@
       <c r="G192" t="s">
         <v>261</v>
       </c>
-      <c r="H192">
+      <c r="H192" s="5">
         <v>2019</v>
       </c>
       <c r="I192">
@@ -14133,7 +14139,7 @@
       <c r="G193" t="s">
         <v>319</v>
       </c>
-      <c r="H193">
+      <c r="H193" s="5">
         <v>2019</v>
       </c>
       <c r="I193">
@@ -14195,7 +14201,7 @@
       <c r="G194" t="s">
         <v>406</v>
       </c>
-      <c r="H194">
+      <c r="H194" s="5">
         <v>2019</v>
       </c>
       <c r="I194">
@@ -14254,7 +14260,7 @@
       <c r="G195" t="s">
         <v>123</v>
       </c>
-      <c r="H195">
+      <c r="H195" s="5">
         <v>2019</v>
       </c>
       <c r="I195">
@@ -14316,7 +14322,7 @@
       <c r="G196" t="s">
         <v>55</v>
       </c>
-      <c r="H196">
+      <c r="H196" s="5">
         <v>2019</v>
       </c>
       <c r="I196">
@@ -14378,7 +14384,7 @@
       <c r="G197" t="s">
         <v>135</v>
       </c>
-      <c r="H197">
+      <c r="H197" s="5">
         <v>2019</v>
       </c>
       <c r="I197">
@@ -14440,7 +14446,7 @@
       <c r="G198" t="s">
         <v>517</v>
       </c>
-      <c r="H198">
+      <c r="H198" s="5">
         <v>2019</v>
       </c>
       <c r="I198">
@@ -14490,7 +14496,7 @@
       <c r="G199" t="s">
         <v>225</v>
       </c>
-      <c r="H199">
+      <c r="H199" s="5">
         <v>2019</v>
       </c>
       <c r="I199">
@@ -14555,7 +14561,7 @@
       <c r="G200" t="s">
         <v>280</v>
       </c>
-      <c r="H200">
+      <c r="H200" s="5">
         <v>2019</v>
       </c>
       <c r="I200">
@@ -14617,7 +14623,7 @@
       <c r="G201" t="s">
         <v>520</v>
       </c>
-      <c r="H201">
+      <c r="H201" s="5">
         <v>2019</v>
       </c>
       <c r="I201">
@@ -14664,7 +14670,7 @@
       <c r="G202" t="s">
         <v>515</v>
       </c>
-      <c r="H202">
+      <c r="H202" s="5">
         <v>2019</v>
       </c>
       <c r="I202">
@@ -14723,7 +14729,7 @@
       <c r="G203" t="s">
         <v>522</v>
       </c>
-      <c r="H203">
+      <c r="H203" s="5">
         <v>2019</v>
       </c>
       <c r="I203">
@@ -14773,7 +14779,7 @@
       <c r="G204" t="s">
         <v>256</v>
       </c>
-      <c r="H204">
+      <c r="H204" s="5">
         <v>2019</v>
       </c>
       <c r="I204">
@@ -14835,7 +14841,7 @@
       <c r="G205" t="s">
         <v>329</v>
       </c>
-      <c r="H205">
+      <c r="H205" s="5">
         <v>2019</v>
       </c>
       <c r="I205">
@@ -14897,7 +14903,7 @@
       <c r="G206" t="s">
         <v>109</v>
       </c>
-      <c r="H206">
+      <c r="H206" s="5">
         <v>2019</v>
       </c>
       <c r="I206">
@@ -14959,7 +14965,7 @@
       <c r="G207" t="s">
         <v>407</v>
       </c>
-      <c r="H207">
+      <c r="H207" s="5">
         <v>2019</v>
       </c>
       <c r="I207">
@@ -15018,7 +15024,7 @@
       <c r="G208" t="s">
         <v>174</v>
       </c>
-      <c r="H208">
+      <c r="H208" s="5">
         <v>2019</v>
       </c>
       <c r="I208">
@@ -15080,7 +15086,7 @@
       <c r="G209" t="s">
         <v>305</v>
       </c>
-      <c r="H209">
+      <c r="H209" s="5">
         <v>2019</v>
       </c>
       <c r="I209">
@@ -15142,7 +15148,7 @@
       <c r="G210" t="s">
         <v>348</v>
       </c>
-      <c r="H210">
+      <c r="H210" s="5">
         <v>2019</v>
       </c>
       <c r="I210">
@@ -15201,7 +15207,7 @@
       <c r="G211" t="s">
         <v>217</v>
       </c>
-      <c r="H211">
+      <c r="H211" s="5">
         <v>2019</v>
       </c>
       <c r="I211">
@@ -15263,7 +15269,7 @@
       <c r="G212" t="s">
         <v>57</v>
       </c>
-      <c r="H212">
+      <c r="H212" s="5">
         <v>2019</v>
       </c>
       <c r="I212">
@@ -15325,7 +15331,7 @@
       <c r="G213" t="s">
         <v>261</v>
       </c>
-      <c r="H213">
+      <c r="H213" s="5">
         <v>2019</v>
       </c>
       <c r="I213">
@@ -15387,7 +15393,7 @@
       <c r="G214" t="s">
         <v>400</v>
       </c>
-      <c r="H214">
+      <c r="H214" s="5">
         <v>2019</v>
       </c>
       <c r="I214">
@@ -15449,7 +15455,7 @@
       <c r="G215" t="s">
         <v>209</v>
       </c>
-      <c r="H215">
+      <c r="H215" s="5">
         <v>2019</v>
       </c>
       <c r="I215">
@@ -15511,7 +15517,7 @@
       <c r="G216" t="s">
         <v>42</v>
       </c>
-      <c r="H216">
+      <c r="H216" s="5">
         <v>2019</v>
       </c>
       <c r="I216">
@@ -15567,7 +15573,7 @@
       <c r="G217" t="s">
         <v>300</v>
       </c>
-      <c r="H217">
+      <c r="H217" s="5">
         <v>2019</v>
       </c>
       <c r="I217">
@@ -15629,7 +15635,7 @@
       <c r="G218" t="s">
         <v>409</v>
       </c>
-      <c r="H218">
+      <c r="H218" s="5">
         <v>2019</v>
       </c>
       <c r="I218">
@@ -15691,7 +15697,7 @@
       <c r="G219" t="s">
         <v>118</v>
       </c>
-      <c r="H219">
+      <c r="H219" s="5">
         <v>2019</v>
       </c>
       <c r="I219">
@@ -15753,7 +15759,7 @@
       <c r="G220" t="s">
         <v>193</v>
       </c>
-      <c r="H220">
+      <c r="H220" s="5">
         <v>2019</v>
       </c>
       <c r="I220">
@@ -15815,7 +15821,7 @@
       <c r="G221" t="s">
         <v>202</v>
       </c>
-      <c r="H221">
+      <c r="H221" s="5">
         <v>2019</v>
       </c>
       <c r="I221">
@@ -15877,7 +15883,7 @@
       <c r="G222" t="s">
         <v>485</v>
       </c>
-      <c r="H222">
+      <c r="H222" s="5">
         <v>2019</v>
       </c>
       <c r="I222">
@@ -15936,7 +15942,7 @@
       <c r="G223" t="s">
         <v>249</v>
       </c>
-      <c r="H223">
+      <c r="H223" s="5">
         <v>2019</v>
       </c>
       <c r="I223">
@@ -15998,7 +16004,7 @@
       <c r="G224" t="s">
         <v>115</v>
       </c>
-      <c r="H224">
+      <c r="H224" s="5">
         <v>2019</v>
       </c>
       <c r="I224">
@@ -16063,7 +16069,7 @@
       <c r="G225" t="s">
         <v>524</v>
       </c>
-      <c r="H225">
+      <c r="H225" s="5">
         <v>2019</v>
       </c>
       <c r="I225">
@@ -16107,7 +16113,7 @@
       <c r="G226" t="s">
         <v>95</v>
       </c>
-      <c r="H226">
+      <c r="H226" s="5">
         <v>2019</v>
       </c>
       <c r="I226">
@@ -16166,7 +16172,7 @@
       <c r="G227" t="s">
         <v>244</v>
       </c>
-      <c r="H227">
+      <c r="H227" s="5">
         <v>2019</v>
       </c>
       <c r="I227">
@@ -16228,7 +16234,7 @@
       <c r="G228" t="s">
         <v>118</v>
       </c>
-      <c r="H228">
+      <c r="H228" s="5">
         <v>2019</v>
       </c>
       <c r="I228">
@@ -16290,7 +16296,7 @@
       <c r="G229" t="s">
         <v>164</v>
       </c>
-      <c r="H229">
+      <c r="H229" s="5">
         <v>2019</v>
       </c>
       <c r="I229">
@@ -16352,7 +16358,7 @@
       <c r="G230" t="s">
         <v>155</v>
       </c>
-      <c r="H230">
+      <c r="H230" s="5">
         <v>2019</v>
       </c>
       <c r="I230">
@@ -16411,7 +16417,7 @@
       <c r="G231" t="s">
         <v>276</v>
       </c>
-      <c r="H231">
+      <c r="H231" s="5">
         <v>2019</v>
       </c>
       <c r="I231">
@@ -16473,7 +16479,7 @@
       <c r="G232" t="s">
         <v>294</v>
       </c>
-      <c r="H232">
+      <c r="H232" s="5">
         <v>2019</v>
       </c>
       <c r="I232">
@@ -16529,7 +16535,7 @@
       <c r="G233" t="s">
         <v>236</v>
       </c>
-      <c r="H233">
+      <c r="H233" s="5">
         <v>2019</v>
       </c>
       <c r="I233">
@@ -16591,7 +16597,7 @@
       <c r="G234" t="s">
         <v>204</v>
       </c>
-      <c r="H234">
+      <c r="H234" s="5">
         <v>2019</v>
       </c>
       <c r="I234">
@@ -16653,7 +16659,7 @@
       <c r="G235" t="s">
         <v>71</v>
       </c>
-      <c r="H235">
+      <c r="H235" s="5">
         <v>2019</v>
       </c>
       <c r="I235">
@@ -16715,7 +16721,7 @@
       <c r="G236" t="s">
         <v>63</v>
       </c>
-      <c r="H236">
+      <c r="H236" s="5">
         <v>2019</v>
       </c>
       <c r="I236">
@@ -16777,7 +16783,7 @@
       <c r="G237" t="s">
         <v>534</v>
       </c>
-      <c r="H237">
+      <c r="H237" s="5">
         <v>2020</v>
       </c>
       <c r="I237">
@@ -16815,7 +16821,7 @@
       <c r="G238" t="s">
         <v>536</v>
       </c>
-      <c r="H238">
+      <c r="H238" s="5">
         <v>2020</v>
       </c>
       <c r="I238">
@@ -16865,7 +16871,7 @@
       <c r="G239" t="s">
         <v>538</v>
       </c>
-      <c r="H239">
+      <c r="H239" s="5">
         <v>2020</v>
       </c>
       <c r="I239">
@@ -16915,7 +16921,7 @@
       <c r="G240" t="s">
         <v>540</v>
       </c>
-      <c r="H240">
+      <c r="H240" s="5">
         <v>2020</v>
       </c>
       <c r="I240">
@@ -16965,7 +16971,7 @@
       <c r="G241" t="s">
         <v>542</v>
       </c>
-      <c r="H241">
+      <c r="H241" s="5">
         <v>2020</v>
       </c>
       <c r="I241">
@@ -17015,7 +17021,7 @@
       <c r="G242" t="s">
         <v>544</v>
       </c>
-      <c r="H242">
+      <c r="H242" s="5">
         <v>2020</v>
       </c>
       <c r="I242">
@@ -17062,7 +17068,7 @@
       <c r="G243" t="s">
         <v>546</v>
       </c>
-      <c r="H243">
+      <c r="H243" s="5">
         <v>2020</v>
       </c>
       <c r="I243">
@@ -17112,7 +17118,7 @@
       <c r="G244" t="s">
         <v>548</v>
       </c>
-      <c r="H244">
+      <c r="H244" s="5">
         <v>2020</v>
       </c>
       <c r="I244">
@@ -17162,7 +17168,7 @@
       <c r="G245" t="s">
         <v>550</v>
       </c>
-      <c r="H245">
+      <c r="H245" s="5">
         <v>2020</v>
       </c>
       <c r="I245">
@@ -17212,7 +17218,7 @@
       <c r="G246" t="s">
         <v>552</v>
       </c>
-      <c r="H246">
+      <c r="H246" s="5">
         <v>2020</v>
       </c>
       <c r="I246">
@@ -17262,7 +17268,7 @@
       <c r="G247" t="s">
         <v>554</v>
       </c>
-      <c r="H247">
+      <c r="H247" s="5">
         <v>2020</v>
       </c>
       <c r="I247">
@@ -17309,7 +17315,7 @@
       <c r="G248" t="s">
         <v>556</v>
       </c>
-      <c r="H248">
+      <c r="H248" s="5">
         <v>2020</v>
       </c>
       <c r="I248">
@@ -17359,7 +17365,7 @@
       <c r="G249" t="s">
         <v>558</v>
       </c>
-      <c r="H249">
+      <c r="H249" s="5">
         <v>2020</v>
       </c>
       <c r="I249">
@@ -17409,7 +17415,7 @@
       <c r="G250" t="s">
         <v>560</v>
       </c>
-      <c r="H250">
+      <c r="H250" s="5">
         <v>2020</v>
       </c>
       <c r="I250">
@@ -17459,7 +17465,7 @@
       <c r="G251" t="s">
         <v>562</v>
       </c>
-      <c r="H251">
+      <c r="H251" s="5">
         <v>2020</v>
       </c>
       <c r="I251">
@@ -17509,7 +17515,7 @@
       <c r="G252" t="s">
         <v>564</v>
       </c>
-      <c r="H252">
+      <c r="H252" s="5">
         <v>2020</v>
       </c>
       <c r="I252">
@@ -17559,7 +17565,7 @@
       <c r="G253" t="s">
         <v>552</v>
       </c>
-      <c r="H253">
+      <c r="H253" s="5">
         <v>2020</v>
       </c>
       <c r="I253">
@@ -17594,7 +17600,7 @@
       <c r="G254" t="s">
         <v>567</v>
       </c>
-      <c r="H254">
+      <c r="H254" s="5">
         <v>2020</v>
       </c>
       <c r="I254">
@@ -17644,7 +17650,7 @@
       <c r="G255" t="s">
         <v>569</v>
       </c>
-      <c r="H255">
+      <c r="H255" s="5">
         <v>2020</v>
       </c>
       <c r="I255">
@@ -17694,7 +17700,7 @@
       <c r="G256" t="s">
         <v>571</v>
       </c>
-      <c r="H256">
+      <c r="H256" s="5">
         <v>2020</v>
       </c>
       <c r="I256">
@@ -17744,7 +17750,7 @@
       <c r="G257" t="s">
         <v>573</v>
       </c>
-      <c r="H257">
+      <c r="H257" s="5">
         <v>2020</v>
       </c>
       <c r="I257">
@@ -17794,7 +17800,7 @@
       <c r="G258" t="s">
         <v>528</v>
       </c>
-      <c r="H258">
+      <c r="H258" s="5">
         <v>2020</v>
       </c>
       <c r="I258">
@@ -17844,7 +17850,7 @@
       <c r="G259" t="s">
         <v>576</v>
       </c>
-      <c r="H259">
+      <c r="H259" s="5">
         <v>2020</v>
       </c>
       <c r="I259">
@@ -17894,7 +17900,7 @@
       <c r="G260" t="s">
         <v>578</v>
       </c>
-      <c r="H260">
+      <c r="H260" s="5">
         <v>2020</v>
       </c>
       <c r="I260">
@@ -17941,7 +17947,7 @@
       <c r="G261" t="s">
         <v>580</v>
       </c>
-      <c r="H261">
+      <c r="H261" s="5">
         <v>2020</v>
       </c>
       <c r="I261">
@@ -17991,7 +17997,7 @@
       <c r="G262" t="s">
         <v>582</v>
       </c>
-      <c r="H262">
+      <c r="H262" s="5">
         <v>2020</v>
       </c>
       <c r="I262">
@@ -18041,7 +18047,7 @@
       <c r="G263" t="s">
         <v>584</v>
       </c>
-      <c r="H263">
+      <c r="H263" s="5">
         <v>2020</v>
       </c>
       <c r="I263">
@@ -18091,7 +18097,7 @@
       <c r="G264" t="s">
         <v>586</v>
       </c>
-      <c r="H264">
+      <c r="H264" s="5">
         <v>2020</v>
       </c>
       <c r="I264">
@@ -18138,7 +18144,7 @@
       <c r="G265" t="s">
         <v>588</v>
       </c>
-      <c r="H265">
+      <c r="H265" s="5">
         <v>2020</v>
       </c>
       <c r="I265">
@@ -18188,7 +18194,7 @@
       <c r="G266" t="s">
         <v>590</v>
       </c>
-      <c r="H266">
+      <c r="H266" s="5">
         <v>2020</v>
       </c>
       <c r="I266">
@@ -18238,7 +18244,7 @@
       <c r="G267" t="s">
         <v>592</v>
       </c>
-      <c r="H267">
+      <c r="H267" s="5">
         <v>2020</v>
       </c>
       <c r="I267">
@@ -18288,7 +18294,7 @@
       <c r="G268" t="s">
         <v>594</v>
       </c>
-      <c r="H268">
+      <c r="H268" s="5">
         <v>2020</v>
       </c>
       <c r="I268">
@@ -18338,7 +18344,7 @@
       <c r="G269" t="s">
         <v>596</v>
       </c>
-      <c r="H269">
+      <c r="H269" s="5">
         <v>2020</v>
       </c>
       <c r="I269">
@@ -18388,7 +18394,7 @@
       <c r="G270" t="s">
         <v>536</v>
       </c>
-      <c r="H270">
+      <c r="H270" s="5">
         <v>2020</v>
       </c>
       <c r="I270">
@@ -18438,7 +18444,7 @@
       <c r="G271" t="s">
         <v>599</v>
       </c>
-      <c r="H271">
+      <c r="H271" s="5">
         <v>2020</v>
       </c>
       <c r="I271">
@@ -18488,7 +18494,7 @@
       <c r="G272" t="s">
         <v>601</v>
       </c>
-      <c r="H272">
+      <c r="H272" s="5">
         <v>2020</v>
       </c>
       <c r="I272">
@@ -18538,7 +18544,7 @@
       <c r="G273" t="s">
         <v>540</v>
       </c>
-      <c r="H273">
+      <c r="H273" s="5">
         <v>2020</v>
       </c>
       <c r="I273">
@@ -18588,7 +18594,7 @@
       <c r="G274" t="s">
         <v>604</v>
       </c>
-      <c r="H274">
+      <c r="H274" s="5">
         <v>2020</v>
       </c>
       <c r="I274">
@@ -18638,7 +18644,7 @@
       <c r="G275" t="s">
         <v>560</v>
       </c>
-      <c r="H275">
+      <c r="H275" s="5">
         <v>2020</v>
       </c>
       <c r="I275">
@@ -18688,7 +18694,7 @@
       <c r="G276" t="s">
         <v>607</v>
       </c>
-      <c r="H276">
+      <c r="H276" s="5">
         <v>2020</v>
       </c>
       <c r="I276">
@@ -18738,7 +18744,7 @@
       <c r="G277" t="s">
         <v>609</v>
       </c>
-      <c r="H277">
+      <c r="H277" s="5">
         <v>2020</v>
       </c>
       <c r="I277">
@@ -18788,7 +18794,7 @@
       <c r="G278" t="s">
         <v>611</v>
       </c>
-      <c r="H278">
+      <c r="H278" s="5">
         <v>2020</v>
       </c>
       <c r="I278">
@@ -18838,7 +18844,7 @@
       <c r="G279" t="s">
         <v>613</v>
       </c>
-      <c r="H279">
+      <c r="H279" s="5">
         <v>2020</v>
       </c>
       <c r="I279">
@@ -18888,7 +18894,7 @@
       <c r="G280" t="s">
         <v>613</v>
       </c>
-      <c r="H280">
+      <c r="H280" s="5">
         <v>2020</v>
       </c>
       <c r="I280">
@@ -18938,7 +18944,7 @@
       <c r="G281" t="s">
         <v>554</v>
       </c>
-      <c r="H281">
+      <c r="H281" s="5">
         <v>2020</v>
       </c>
       <c r="I281">
@@ -18988,7 +18994,7 @@
       <c r="G282" t="s">
         <v>617</v>
       </c>
-      <c r="H282">
+      <c r="H282" s="5">
         <v>2020</v>
       </c>
       <c r="I282">
@@ -19038,7 +19044,7 @@
       <c r="G283" t="s">
         <v>619</v>
       </c>
-      <c r="H283">
+      <c r="H283" s="5">
         <v>2020</v>
       </c>
       <c r="I283">
@@ -19088,7 +19094,7 @@
       <c r="G284" t="s">
         <v>621</v>
       </c>
-      <c r="H284">
+      <c r="H284" s="5">
         <v>2020</v>
       </c>
       <c r="I284">
@@ -19138,7 +19144,7 @@
       <c r="G285" t="s">
         <v>623</v>
       </c>
-      <c r="H285">
+      <c r="H285" s="5">
         <v>2020</v>
       </c>
       <c r="I285">
@@ -19188,7 +19194,7 @@
       <c r="G286" t="s">
         <v>625</v>
       </c>
-      <c r="H286">
+      <c r="H286" s="5">
         <v>2020</v>
       </c>
       <c r="I286">
@@ -19238,7 +19244,7 @@
       <c r="G287" t="s">
         <v>223</v>
       </c>
-      <c r="H287">
+      <c r="H287" s="5">
         <v>2020</v>
       </c>
       <c r="I287">
@@ -19288,7 +19294,7 @@
       <c r="G288" t="s">
         <v>628</v>
       </c>
-      <c r="H288">
+      <c r="H288" s="5">
         <v>2020</v>
       </c>
       <c r="I288">
@@ -19335,7 +19341,7 @@
       <c r="G289" t="s">
         <v>630</v>
       </c>
-      <c r="H289">
+      <c r="H289" s="5">
         <v>2020</v>
       </c>
       <c r="I289">

</xml_diff>

<commit_message>
closer. now next need to fix the median vs. average
</commit_message>
<xml_diff>
--- a/Shiny_app/FDA_Drug_Trials_Snapshots_2015-20.xlsx
+++ b/Shiny_app/FDA_Drug_Trials_Snapshots_2015-20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Documents/GitHub/FDA_DTS/Shiny_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A536ABD-5BEE-8B45-9886-D5BFFC4729AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE783FF-9BBD-DC4F-ADC7-298D514BDBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3707,8 +3707,8 @@
   <dimension ref="A1:X289"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17445,7 +17445,7 @@
         <v>699</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>630</v>
+        <v>162</v>
       </c>
       <c r="E251" s="3" t="s">
         <v>630</v>

</xml_diff>

<commit_message>
summary statistics works for 1 table
</commit_message>
<xml_diff>
--- a/Shiny_app/FDA_Drug_Trials_Snapshots_2015-20.xlsx
+++ b/Shiny_app/FDA_Drug_Trials_Snapshots_2015-20.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arielcarmeli/Documents/GitHub/FDA_DTS/Shiny_app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE783FF-9BBD-DC4F-ADC7-298D514BDBB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E77083F7-08B0-BC44-B29A-1002C05969D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3704,11 +3704,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:X289"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N39" sqref="N39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4308,7 +4309,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>529</v>
       </c>
@@ -6722,7 +6723,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>430</v>
       </c>
@@ -6769,7 +6770,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>440</v>
       </c>
@@ -6816,7 +6817,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>168</v>
       </c>
@@ -6863,7 +6864,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>140</v>
       </c>
@@ -6910,7 +6911,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>432</v>
       </c>
@@ -6957,7 +6958,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>486</v>
       </c>
@@ -7004,7 +7005,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>105</v>
       </c>
@@ -7051,7 +7052,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>296</v>
       </c>
@@ -7098,7 +7099,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>506</v>
       </c>
@@ -7145,7 +7146,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>331</v>
       </c>
@@ -7192,7 +7193,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>333</v>
       </c>
@@ -7239,7 +7240,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>78</v>
       </c>
@@ -7286,7 +7287,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>527</v>
       </c>
@@ -7321,7 +7322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>369</v>
       </c>
@@ -7371,7 +7372,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>372</v>
       </c>
@@ -7418,7 +7419,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>348</v>
       </c>
@@ -7465,7 +7466,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>634</v>
       </c>
@@ -7512,7 +7513,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>413</v>
       </c>
@@ -7559,7 +7560,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>350</v>
       </c>
@@ -7606,7 +7607,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>217</v>
       </c>
@@ -7653,7 +7654,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>476</v>
       </c>
@@ -7700,7 +7701,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>181</v>
       </c>
@@ -7747,7 +7748,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>374</v>
       </c>
@@ -7794,7 +7795,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>315</v>
       </c>
@@ -7841,7 +7842,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>466</v>
       </c>
@@ -7891,7 +7892,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>401</v>
       </c>
@@ -7938,7 +7939,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>37</v>
       </c>
@@ -7988,7 +7989,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>472</v>
       </c>
@@ -8038,7 +8039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>305</v>
       </c>
@@ -8088,7 +8089,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>525</v>
       </c>
@@ -8126,7 +8127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>264</v>
       </c>
@@ -8173,7 +8174,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>213</v>
       </c>
@@ -8223,7 +8224,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>119</v>
       </c>
@@ -8273,7 +8274,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="91" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>155</v>
       </c>
@@ -8323,7 +8324,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>125</v>
       </c>
@@ -8373,7 +8374,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>329</v>
       </c>
@@ -8417,7 +8418,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>633</v>
       </c>
@@ -8467,7 +8468,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>256</v>
       </c>
@@ -8520,7 +8521,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>232</v>
       </c>
@@ -8570,7 +8571,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -8620,7 +8621,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>209</v>
       </c>
@@ -8667,7 +8668,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>307</v>
       </c>
@@ -8717,7 +8718,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>319</v>
       </c>
@@ -8767,7 +8768,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>187</v>
       </c>
@@ -8817,7 +8818,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>410</v>
       </c>
@@ -8864,7 +8865,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>271</v>
       </c>
@@ -8914,7 +8915,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>322</v>
       </c>
@@ -8964,7 +8965,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>143</v>
       </c>
@@ -9014,7 +9015,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>220</v>
       </c>
@@ -9064,7 +9065,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>261</v>
       </c>
@@ -9114,7 +9115,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>240</v>
       </c>
@@ -9164,7 +9165,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>452</v>
       </c>
@@ -9214,7 +9215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>20</v>
       </c>
@@ -9264,7 +9265,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>280</v>
       </c>
@@ -9314,7 +9315,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>230</v>
       </c>
@@ -9364,7 +9365,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>230</v>
       </c>
@@ -9414,7 +9415,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>425</v>
       </c>
@@ -9461,7 +9462,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>76</v>
       </c>
@@ -9511,7 +9512,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>291</v>
       </c>
@@ -9561,7 +9562,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>185</v>
       </c>
@@ -9611,7 +9612,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>157</v>
       </c>
@@ -9661,7 +9662,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>321</v>
       </c>
@@ -9711,7 +9712,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>289</v>
       </c>
@@ -9761,7 +9762,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>496</v>
       </c>
@@ -9811,7 +9812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>246</v>
       </c>
@@ -9861,7 +9862,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>195</v>
       </c>
@@ -9911,7 +9912,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>236</v>
       </c>
@@ -9961,7 +9962,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>57</v>
       </c>
@@ -10011,7 +10012,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>80</v>
       </c>
@@ -10061,7 +10062,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>32</v>
       </c>
@@ -10114,7 +10115,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>367</v>
       </c>
@@ -10164,7 +10165,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>460</v>
       </c>
@@ -10226,7 +10227,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>166</v>
       </c>
@@ -10288,7 +10289,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>212</v>
       </c>
@@ -10350,7 +10351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="132" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>356</v>
       </c>
@@ -10412,7 +10413,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>311</v>
       </c>
@@ -10474,7 +10475,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>123</v>
       </c>
@@ -10536,7 +10537,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>138</v>
       </c>
@@ -10598,7 +10599,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>478</v>
       </c>
@@ -10660,7 +10661,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>189</v>
       </c>
@@ -10722,7 +10723,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>178</v>
       </c>
@@ -10784,7 +10785,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>408</v>
       </c>
@@ -10843,7 +10844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>523</v>
       </c>
@@ -10893,7 +10894,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>276</v>
       </c>
@@ -10955,7 +10956,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>632</v>
       </c>
@@ -11017,7 +11018,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>286</v>
       </c>
@@ -11079,7 +11080,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>73</v>
       </c>
@@ -11141,7 +11142,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="145" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>84</v>
       </c>
@@ -11203,7 +11204,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="146" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>238</v>
       </c>
@@ -11265,7 +11266,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="147" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -11327,7 +11328,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="148" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>474</v>
       </c>
@@ -11386,7 +11387,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="149" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>193</v>
       </c>
@@ -11448,7 +11449,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="150" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>225</v>
       </c>
@@ -11510,7 +11511,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="151" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>364</v>
       </c>
@@ -11572,7 +11573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>313</v>
       </c>
@@ -11634,7 +11635,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="153" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>423</v>
       </c>
@@ -11693,7 +11694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="154" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>267</v>
       </c>
@@ -11758,7 +11759,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="155" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>399</v>
       </c>
@@ -11820,7 +11821,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="156" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>135</v>
       </c>
@@ -11882,7 +11883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>489</v>
       </c>
@@ -11944,7 +11945,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>421</v>
       </c>
@@ -12003,7 +12004,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="159" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>42</v>
       </c>
@@ -12065,7 +12066,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>174</v>
       </c>
@@ -12127,7 +12128,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="161" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>376</v>
       </c>
@@ -12189,7 +12190,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>448</v>
       </c>
@@ -12251,7 +12252,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="163" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>294</v>
       </c>
@@ -12313,7 +12314,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="164" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>283</v>
       </c>
@@ -12378,7 +12379,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="165" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>228</v>
       </c>
@@ -12440,7 +12441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="166" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>251</v>
       </c>
@@ -12502,7 +12503,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="167" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>204</v>
       </c>
@@ -12561,7 +12562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="168" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>88</v>
       </c>
@@ -12623,7 +12624,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="169" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>176</v>
       </c>
@@ -12685,7 +12686,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="170" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>64</v>
       </c>
@@ -12747,7 +12748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="171" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>309</v>
       </c>
@@ -12809,7 +12810,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="172" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>300</v>
       </c>
@@ -12871,7 +12872,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="173" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>92</v>
       </c>
@@ -12933,7 +12934,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="174" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>128</v>
       </c>
@@ -12998,7 +12999,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="175" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>197</v>
       </c>
@@ -13060,7 +13061,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>97</v>
       </c>
@@ -13122,7 +13123,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="177" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>244</v>
       </c>
@@ -13184,7 +13185,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="178" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>100</v>
       </c>
@@ -13246,7 +13247,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="179" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>149</v>
       </c>
@@ -13308,7 +13309,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="180" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>95</v>
       </c>
@@ -13370,7 +13371,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>159</v>
       </c>
@@ -13432,7 +13433,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="182" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>71</v>
       </c>
@@ -13494,7 +13495,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>361</v>
       </c>
@@ -13556,7 +13557,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="184" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>454</v>
       </c>
@@ -13618,7 +13619,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="185" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>287</v>
       </c>
@@ -13680,7 +13681,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>109</v>
       </c>
@@ -13742,7 +13743,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="187" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>131</v>
       </c>
@@ -13804,7 +13805,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="188" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>510</v>
       </c>
@@ -13866,7 +13867,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="189" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>164</v>
       </c>
@@ -13928,7 +13929,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="190" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>25</v>
       </c>
@@ -13987,7 +13988,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="191" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>183</v>
       </c>
@@ -14049,7 +14050,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="192" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>259</v>
       </c>
@@ -14111,7 +14112,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="193" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>317</v>
       </c>
@@ -14173,7 +14174,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="194" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>403</v>
       </c>
@@ -14232,7 +14233,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="195" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>121</v>
       </c>
@@ -14294,7 +14295,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="196" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>51</v>
       </c>
@@ -14356,7 +14357,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>133</v>
       </c>
@@ -14418,7 +14419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="198" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>514</v>
       </c>
@@ -14468,7 +14469,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="199" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>223</v>
       </c>
@@ -14530,7 +14531,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="200" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>277</v>
       </c>
@@ -14595,7 +14596,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="201" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>517</v>
       </c>
@@ -14642,7 +14643,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="202" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>512</v>
       </c>
@@ -14701,7 +14702,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="203" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>519</v>
       </c>
@@ -14751,7 +14752,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="204" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>253</v>
       </c>
@@ -14813,7 +14814,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="205" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>327</v>
       </c>
@@ -14875,7 +14876,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>107</v>
       </c>
@@ -14937,7 +14938,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="207" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>631</v>
       </c>
@@ -14996,7 +14997,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>172</v>
       </c>
@@ -15058,7 +15059,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="209" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>303</v>
       </c>
@@ -15120,7 +15121,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>346</v>
       </c>
@@ -15179,7 +15180,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="211" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>215</v>
       </c>
@@ -15241,7 +15242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="212" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>55</v>
       </c>
@@ -15303,7 +15304,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="213" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>266</v>
       </c>
@@ -15365,7 +15366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>397</v>
       </c>
@@ -15427,7 +15428,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="215" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>207</v>
       </c>
@@ -15489,7 +15490,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="216" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>39</v>
       </c>
@@ -15545,7 +15546,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="217" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>298</v>
       </c>
@@ -15607,7 +15608,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="218" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>406</v>
       </c>
@@ -15669,7 +15670,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="219" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>115</v>
       </c>
@@ -15731,7 +15732,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="220" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>191</v>
       </c>
@@ -15793,7 +15794,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="221" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>199</v>
       </c>
@@ -15855,7 +15856,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="222" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>482</v>
       </c>
@@ -15914,7 +15915,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="223" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>247</v>
       </c>
@@ -15976,7 +15977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="224" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>112</v>
       </c>
@@ -16038,7 +16039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="225" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>521</v>
       </c>
@@ -16085,7 +16086,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="226" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>302</v>
       </c>
@@ -16144,7 +16145,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="227" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>242</v>
       </c>
@@ -16206,7 +16207,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="228" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>148</v>
       </c>
@@ -16268,7 +16269,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="229" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>161</v>
       </c>
@@ -16330,7 +16331,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="230" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>151</v>
       </c>
@@ -16389,7 +16390,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="231" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>273</v>
       </c>
@@ -16451,7 +16452,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="232" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>292</v>
       </c>
@@ -16507,7 +16508,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="233" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>234</v>
       </c>
@@ -16569,7 +16570,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="234" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>202</v>
       </c>
@@ -16631,7 +16632,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="235" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>118</v>
       </c>
@@ -16693,7 +16694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="236" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>60</v>
       </c>
@@ -16755,7 +16756,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="237" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>531</v>
       </c>
@@ -16793,7 +16794,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="238" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>533</v>
       </c>
@@ -16843,7 +16844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="239" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>535</v>
       </c>
@@ -16893,7 +16894,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="240" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>537</v>
       </c>
@@ -16943,7 +16944,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="241" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>539</v>
       </c>
@@ -16993,7 +16994,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="242" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>541</v>
       </c>
@@ -17040,7 +17041,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="243" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>543</v>
       </c>
@@ -17090,7 +17091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="244" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>545</v>
       </c>
@@ -17140,7 +17141,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="245" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>547</v>
       </c>
@@ -17190,7 +17191,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="246" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>549</v>
       </c>
@@ -17218,18 +17219,6 @@
       <c r="N246">
         <v>54</v>
       </c>
-      <c r="O246">
-        <v>0</v>
-      </c>
-      <c r="P246">
-        <v>0</v>
-      </c>
-      <c r="Q246">
-        <v>0</v>
-      </c>
-      <c r="R246">
-        <v>0</v>
-      </c>
       <c r="T246">
         <v>3</v>
       </c>
@@ -17240,7 +17229,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="247" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>551</v>
       </c>
@@ -17287,7 +17276,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="248" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>553</v>
       </c>
@@ -17337,7 +17326,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="249" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>555</v>
       </c>
@@ -17387,7 +17376,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="250" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>557</v>
       </c>
@@ -17437,7 +17426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="251" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>559</v>
       </c>
@@ -17487,7 +17476,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="252" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>561</v>
       </c>
@@ -17537,7 +17526,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="253" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>563</v>
       </c>
@@ -17572,7 +17561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="254" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>564</v>
       </c>
@@ -17622,7 +17611,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="255" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>566</v>
       </c>
@@ -17672,7 +17661,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="256" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>568</v>
       </c>
@@ -17722,7 +17711,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="257" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>570</v>
       </c>
@@ -17772,7 +17761,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="258" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>572</v>
       </c>
@@ -17822,7 +17811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="259" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>573</v>
       </c>
@@ -17872,7 +17861,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="260" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>575</v>
       </c>
@@ -17919,7 +17908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="261" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>577</v>
       </c>
@@ -17969,7 +17958,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="262" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>579</v>
       </c>
@@ -18019,7 +18008,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="263" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>581</v>
       </c>
@@ -18069,7 +18058,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="264" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>583</v>
       </c>
@@ -18116,7 +18105,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="265" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>585</v>
       </c>
@@ -18166,7 +18155,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="266" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>587</v>
       </c>
@@ -18216,7 +18205,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="267" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>589</v>
       </c>
@@ -18266,7 +18255,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="268" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>591</v>
       </c>
@@ -18316,7 +18305,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="269" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>593</v>
       </c>
@@ -18366,7 +18355,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="270" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>595</v>
       </c>
@@ -18416,7 +18405,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="271" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>596</v>
       </c>
@@ -18466,7 +18455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="272" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>598</v>
       </c>
@@ -18516,7 +18505,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="273" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>600</v>
       </c>
@@ -18566,7 +18555,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="274" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>601</v>
       </c>
@@ -18616,7 +18605,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="275" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>603</v>
       </c>
@@ -18666,7 +18655,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="276" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>604</v>
       </c>
@@ -18716,7 +18705,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="277" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>606</v>
       </c>
@@ -18766,7 +18755,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="278" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>608</v>
       </c>
@@ -18816,7 +18805,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="279" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>610</v>
       </c>
@@ -18866,7 +18855,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="280" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>612</v>
       </c>
@@ -18916,7 +18905,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="281" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>613</v>
       </c>
@@ -18966,7 +18955,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="282" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>614</v>
       </c>
@@ -19016,7 +19005,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="283" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>616</v>
       </c>
@@ -19066,7 +19055,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="284" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>618</v>
       </c>
@@ -19116,7 +19105,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="285" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>620</v>
       </c>
@@ -19166,7 +19155,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="286" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>622</v>
       </c>
@@ -19216,7 +19205,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="287" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>624</v>
       </c>
@@ -19266,7 +19255,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="288" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>625</v>
       </c>
@@ -19313,7 +19302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="289" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:24" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>627</v>
       </c>
@@ -19353,6 +19342,16 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:X289" xr:uid="{8273B0B7-75AB-7043-A5E1-1E193EA41E1D}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="2015"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="15">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X289">
       <sortCondition ref="H1:H289"/>
     </sortState>

</xml_diff>